<commit_message>
trying to get all the data in
</commit_message>
<xml_diff>
--- a/Documents/Links.xlsx
+++ b/Documents/Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JD\Documents\College\StateParks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JD\Documents\GitHub\StateParks\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94716878-7032-4A77-8A8D-73863C22DF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3022944-AB6E-4613-B7B0-B9C4128862C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{D0F8C2E3-B881-4614-A8FF-B8F862928A8D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>Albany, Gentry County, MO</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>Some Percipation data</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -645,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3825F18E-200C-4225-B452-088A38DBED61}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -658,366 +667,377 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" t="s">
-        <v>20</v>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
+      <c r="C18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" t="s">
-        <v>35</v>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>37</v>
+      <c r="C20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" t="s">
-        <v>39</v>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
+      <c r="C25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" t="s">
-        <v>49</v>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{4590078C-7B1A-4F9E-8875-EC7D7085CDCE}"/>
-    <hyperlink ref="C1" r:id="rId2" xr:uid="{3CC7048E-C5E2-48A0-A25D-9BE6FE9BE181}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{0DDC0956-2D8F-4C4A-8EF3-218B6DD54F52}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{6C508050-9B86-48E4-8F9F-FD235144589D}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{513D8681-FDEA-4B1B-833B-4EFCC4F5BDBD}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{932BBE91-5EB6-4805-AFF0-84D3F4BBAB4D}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{218176E7-20F5-4A36-879D-649595C0F3DB}"/>
-    <hyperlink ref="C18" r:id="rId8" xr:uid="{CB7DB6B4-A6D9-49E5-AF2D-3B82F15E9AB6}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{545F68E1-ABE1-4D8A-A713-B100A70D290A}"/>
-    <hyperlink ref="C25" r:id="rId10" xr:uid="{B4BEC612-5F24-404A-A151-DBC5A664A42E}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{34238BBD-A632-4BB2-BAA1-1C2C26FD2873}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{4590078C-7B1A-4F9E-8875-EC7D7085CDCE}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{3CC7048E-C5E2-48A0-A25D-9BE6FE9BE181}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{0DDC0956-2D8F-4C4A-8EF3-218B6DD54F52}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{6C508050-9B86-48E4-8F9F-FD235144589D}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{513D8681-FDEA-4B1B-833B-4EFCC4F5BDBD}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{932BBE91-5EB6-4805-AFF0-84D3F4BBAB4D}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{218176E7-20F5-4A36-879D-649595C0F3DB}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{CB7DB6B4-A6D9-49E5-AF2D-3B82F15E9AB6}"/>
+    <hyperlink ref="C21" r:id="rId9" xr:uid="{545F68E1-ABE1-4D8A-A713-B100A70D290A}"/>
+    <hyperlink ref="C26" r:id="rId10" xr:uid="{B4BEC612-5F24-404A-A151-DBC5A664A42E}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{34238BBD-A632-4BB2-BAA1-1C2C26FD2873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>